<commit_message>
and we are back to 0.5xcorr + 2xmmc
</commit_message>
<xml_diff>
--- a/Optimize-Me-30nov2023.xlsx
+++ b/Optimize-Me-30nov2023.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/boris/BVS/numerai/public/numerai-vladthestaker/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\boris\BVS\numerai\public\numerai-vladthestaker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4769399F-97F8-A544-BB2A-14F0EE1AD7A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7147218A-9605-4D02-8FB7-0F9D7E10DA53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>ModelName</t>
   </si>
@@ -159,6 +159,9 @@
   </si>
   <si>
     <t>V42_LGBM_AGNES20</t>
+  </si>
+  <si>
+    <t>V42_TEAGER_ENSEMBLE</t>
   </si>
 </sst>
 </file>
@@ -484,20 +487,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C39"/>
+  <dimension ref="A1:C40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" zoomScale="178" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.5" customWidth="1"/>
-    <col min="2" max="2" width="11.83203125" customWidth="1"/>
-    <col min="3" max="3" width="17.33203125" customWidth="1"/>
+    <col min="1" max="1" width="21.453125" customWidth="1"/>
+    <col min="2" max="2" width="11.81640625" customWidth="1"/>
+    <col min="3" max="3" width="17.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -508,7 +511,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -519,7 +522,7 @@
         <v>15.196</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -530,7 +533,7 @@
         <v>11.704000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -541,7 +544,7 @@
         <v>6.6669999999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -552,7 +555,7 @@
         <v>6.609</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -563,7 +566,7 @@
         <v>6.5730000000000004</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -574,7 +577,7 @@
         <v>6.3810000000000002</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -585,7 +588,7 @@
         <v>6.3150000000000004</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -596,7 +599,7 @@
         <v>6.2830000000000004</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -607,7 +610,7 @@
         <v>6.2450000000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -618,7 +621,7 @@
         <v>6.2309999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -629,7 +632,7 @@
         <v>6.1210000000000004</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -640,7 +643,7 @@
         <v>6.0940000000000003</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -651,7 +654,7 @@
         <v>6.0880000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -662,7 +665,7 @@
         <v>6.024</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -673,7 +676,7 @@
         <v>5.9909999999999997</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -684,7 +687,7 @@
         <v>5.9359999999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -695,7 +698,7 @@
         <v>5.9050000000000002</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -706,7 +709,7 @@
         <v>5.7370000000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -717,7 +720,7 @@
         <v>5.2519999999999998</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -728,7 +731,7 @@
         <v>5.1479999999999997</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -739,7 +742,7 @@
         <v>1.0940000000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -750,7 +753,7 @@
         <v>1.008</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -761,7 +764,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -772,7 +775,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>27</v>
       </c>
@@ -783,7 +786,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>28</v>
       </c>
@@ -794,7 +797,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>29</v>
       </c>
@@ -805,7 +808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>30</v>
       </c>
@@ -816,7 +819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>31</v>
       </c>
@@ -827,7 +830,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>32</v>
       </c>
@@ -838,7 +841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>33</v>
       </c>
@@ -849,7 +852,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>34</v>
       </c>
@@ -860,7 +863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>35</v>
       </c>
@@ -871,7 +874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>36</v>
       </c>
@@ -882,7 +885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>40</v>
       </c>
@@ -893,7 +896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>37</v>
       </c>
@@ -904,7 +907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>38</v>
       </c>
@@ -915,7 +918,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>39</v>
       </c>
@@ -923,6 +926,17 @@
         <v>339</v>
       </c>
       <c r="C39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A40" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B40">
+        <v>339</v>
+      </c>
+      <c r="C40">
         <v>0</v>
       </c>
     </row>

</xml_diff>